<commit_message>
adding updated spreadsheet to repo
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedlehr/Documents/Texas State/CS3398/Common Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2BAA8C-A547-6B45-BDAC-0BDAC9667023}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FDD977-8C0D-6343-B2F9-940B92556E40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="660" windowWidth="23640" windowHeight="13540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Must Have</t>
   </si>
@@ -43,54 +43,6 @@
   </si>
   <si>
     <t>Won't Have</t>
-  </si>
-  <si>
-    <t>Display a list of open bike racks</t>
-  </si>
-  <si>
-    <t>Search function for open bike racks near my destination</t>
-  </si>
-  <si>
-    <t>Ability to reserve a location on a bike rack.</t>
-  </si>
-  <si>
-    <t>Whether the bike racks are lighted at night</t>
-  </si>
-  <si>
-    <t>Ability to report the number of open slots on a bike rack.</t>
-  </si>
-  <si>
-    <t>Ability to report the typical times a bike rack has at least one open slot.</t>
-  </si>
-  <si>
-    <t>Explosions</t>
-  </si>
-  <si>
-    <t>Success includes others achieving their goals</t>
-  </si>
-  <si>
-    <t>Blood, gore and flying bullets</t>
-  </si>
-  <si>
-    <t>Ability for me to walk away and the team still succeeds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saving something valuable together like trees or historic sites. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Building something (virtually) physical together </t>
-  </si>
-  <si>
-    <t>Engineering formulas</t>
-  </si>
-  <si>
-    <t>Options that benefit and hurt others to different degrees.</t>
-  </si>
-  <si>
-    <t>Beautiful avatars that distract me.</t>
-  </si>
-  <si>
-    <t>Historical information and context</t>
   </si>
   <si>
     <r>
@@ -230,6 +182,79 @@
     <t>Qualities you want your stories to have…..</t>
   </si>
   <si>
+    <t>Author(s)</t>
+  </si>
+  <si>
+    <t>Functional Components and Features of the Story</t>
+  </si>
+  <si>
+    <t>Planning Poker Ratings for Story</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Difficulty 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(Hi -&gt; More Difficult)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority/Interest
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(Hi -&gt; More Interest)</t>
+    </r>
+  </si>
+  <si>
+    <t>Project User Stories and Functional Requirements</t>
+  </si>
+  <si>
+    <t>Derivative/Integral Caluculator to assist students who may be struggling with Caulculus or higher level math courses.</t>
+  </si>
+  <si>
+    <t>Sam Pugh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A parking simulating applications for students who have difficulty finding parking in and around campus. Prioritizing by time which lots will be open at any time to allow for efficient searching for parking in areas that may be less full at certain times in the day compared to others. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Physics simiulator with graphical representation of how various physics concepts apply and how the variables are dependent on each other in some cases. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wifi Password Cracker that can be used to test wireless passwords and ensure they are secure enough to avoid others from connecting and stealing wireless internet. </t>
+  </si>
+  <si>
+    <t>Shelby J</t>
+  </si>
+  <si>
+    <t>Efficient Methods to make calculations.</t>
+  </si>
+  <si>
+    <t>Beautiful UI Interface dependent on calculations from sliding bars indicating values.</t>
+  </si>
+  <si>
+    <t>Ability to modify values on the fly to see the changes in real time.</t>
+  </si>
+  <si>
+    <t>Methods showing the steps that are taking place throughout the calculations.</t>
+  </si>
+  <si>
+    <t>A Gui with buttons and ways for the end user to input the inforamtion.</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">List Team Members Here: </t>
     </r>
@@ -241,103 +266,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Mireya Millano, Joe Jones, Kabine Kisoso, etc.</t>
-    </r>
-  </si>
-  <si>
-    <t>Socially redeeming features?</t>
-  </si>
-  <si>
-    <t>Complicated social and ethical challenges</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Example (please delete after reviewing)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: I, Joe, as a student of Texas State University would like to be able to find open bike racks on campus before I come to campus so that I don't waste my time looking.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Example (please delete after reviewing):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> As an almost 60 year old,  feeling out of touch with the world, I would like to learn a video game that doesn't include things that blow up.</t>
-    </r>
-  </si>
-  <si>
-    <t>Author(s)</t>
-  </si>
-  <si>
-    <t>Functional Components and Features of the Story</t>
-  </si>
-  <si>
-    <t>Planning Poker Ratings for Story</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Difficulty 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>(Hi -&gt; More Difficult)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Priority/Interest
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>(Hi -&gt; More Interest)</t>
-    </r>
-  </si>
-  <si>
-    <t>&lt;Your Team's Project Name&gt;</t>
-  </si>
-  <si>
-    <t>Project User Stories and Functional Requirements</t>
+      <t xml:space="preserve">Sam Pugh, </t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;CS3398 Kree Playing Poker Project Discussion&gt;</t>
+  </si>
+  <si>
+    <t>Calculation Engine that can evaulate derivatives and integrals depending on settings specified by the user.</t>
   </si>
 </sst>
 </file>
@@ -714,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -755,60 +691,66 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,7 +1048,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1123,47 +1065,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="42" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="25"/>
+      <c r="A1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="A2" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="34"/>
+      <c r="E2" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="45" thickTop="1" thickBot="1">
-      <c r="A3" s="26"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="12" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>0</v>
@@ -1178,137 +1120,131 @@
         <v>3</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="146" thickTop="1" thickBot="1">
+      <c r="A4" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="13">
+        <v>34</v>
+      </c>
+      <c r="D4" s="13">
+        <v>34</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="36" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="146" thickTop="1" thickBot="1">
-      <c r="A4" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="7" t="s">
+      <c r="H4" s="7"/>
+      <c r="J4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="66" thickTop="1" thickBot="1">
-      <c r="A5" s="21"/>
-      <c r="B5" s="18"/>
+    </row>
+    <row r="5" spans="1:10" ht="17" thickTop="1" thickBot="1">
+      <c r="A5" s="31"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="48">
-      <c r="A6" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="17"/>
+    <row r="6" spans="1:10">
+      <c r="A6" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="16"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
-      <c r="E6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="64">
-      <c r="A7" s="23"/>
-      <c r="B7" s="17"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" ht="16">
+      <c r="A7" s="21"/>
+      <c r="B7" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="64">
-      <c r="A8" s="24"/>
-      <c r="B8" s="19"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="22"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="150" customHeight="1" thickBot="1">
+      <c r="A9" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="F9" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="16" thickBot="1">
+      <c r="A10" s="31"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="150" customHeight="1" thickBot="1">
+      <c r="A11" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="16" thickBot="1">
+      <c r="A12" s="31"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:10">
       <c r="B13" s="3"/>
@@ -1383,14 +1319,16 @@
       <c r="H20" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added name to top of file.
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -44,7 +44,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Sam Pugh, David Kim, </t>
+      <t xml:space="preserve">Sam Pugh, David Kim, Shelby Jordan,</t>
     </r>
   </si>
   <si>
@@ -342,7 +342,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -410,12 +410,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF262626"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -560,7 +554,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,10 +575,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -639,10 +629,6 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -724,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -743,7 +729,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -754,242 +740,241 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
       <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" s="10" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+    <row r="2" s="9" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" s="10" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="11" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" s="9" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="146" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="14" t="n">
         <v>34</v>
       </c>
-      <c r="D4" s="15" t="n">
+      <c r="D4" s="14" t="n">
         <v>34</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="J4" s="18" t="s">
+      <c r="H4" s="16"/>
+      <c r="J4" s="17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="15" t="n">
+      <c r="C6" s="14" t="n">
         <v>55</v>
       </c>
-      <c r="D6" s="15" t="n">
+      <c r="D6" s="14" t="n">
         <v>55</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15" t="n">
+      <c r="C9" s="14" t="n">
         <v>55</v>
       </c>
-      <c r="D9" s="15" t="n">
+      <c r="D9" s="14" t="n">
         <v>34</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="15" t="n">
+      <c r="C11" s="14" t="n">
         <v>34</v>
       </c>
-      <c r="D11" s="15" t="n">
+      <c r="D11" s="14" t="n">
         <v>34</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="157" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="15" t="n">
+      <c r="C13" s="14" t="n">
         <v>34</v>
       </c>
-      <c r="D13" s="15" t="n">
+      <c r="D13" s="14" t="n">
         <v>55</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
finished assignment file, Adding additional must have, should have etc fields
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D566018C-3B4A-2841-BDDF-EAC4DBA286EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B4A163-BC4C-C443-AB38-5C9055B2788F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,21 +597,6 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -633,20 +618,35 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1033,12 +1033,12 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
@@ -1051,323 +1051,328 @@
     <col min="11" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" ht="42" customHeight="1" thickBot="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="42" customHeight="1" thickBot="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" s="10" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="J2" s="8" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="J2" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="10" customFormat="1" ht="45" thickTop="1" thickBot="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="11" t="s">
+    <row r="3" spans="1:10" s="5" customFormat="1" ht="45" thickTop="1" thickBot="1">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="146" customHeight="1">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="11">
         <v>34</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="11">
         <v>34</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="J4" s="13" t="s">
+      <c r="H4" s="9"/>
+      <c r="J4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="150" customHeight="1">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="11">
         <v>55</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="11">
         <v>55</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="150" customHeight="1">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="11">
         <v>55</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="11">
         <v>34</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="14"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:10" ht="150" customHeight="1">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="11">
         <v>34</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="11">
         <v>34</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:10" ht="157" customHeight="1">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:10" ht="150" customHeight="1">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" ht="150" customHeight="1">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="14" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:H2"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A4:A5"/>
@@ -1375,11 +1380,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Sam Finished his part of spreadsheet and added 2 should and could have fields for each story
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FF1595-3973-C849-8080-D66FCCA95CC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCEB112-2123-C644-B42F-6330E81FFDDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>&lt;CS3398 Kree Playing Poker Project Discussion&gt;</t>
   </si>
@@ -399,13 +399,31 @@
     <t>I Sam, as a Mathematics , major have difficulties and struggle when first attempting to solve Calculus equations.This  Derivative/Integral Caluculator is meant to assist those who need to see step by step procedures in order to better understand the process which the</t>
   </si>
   <si>
-    <t xml:space="preserve">I Sam, as a user who must take Physics to obtain my degree have trouble because the Fundementals of Physics can be  frusterating for students who tend to be visual learners. This web application is meant to alleviate those troubles by adding graphics to the calculations to help students visualize the concepts by seeing graphics of how interactions of objects occur and the different forces/energies that they interact with as well as the objects themselves. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Must be integrated within a web application. </t>
   </si>
   <si>
     <t>Additional resource options if the student does not understand the steps.</t>
+  </si>
+  <si>
+    <t>Happy brithday playing whenever you git the calculate button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I Sam, as a user who must take Physics to obtain my degree have trouble because the fundementals of Physics can be  frusterating for students who tend to be visual learners. This web application is meant to alleviate those troubles by adding graphics to the calculations to help students visualize the concepts by seeing graphics of how interactions of objects occur and the different forces/energies that they interact with as well as the objects themselves. </t>
+  </si>
+  <si>
+    <t>An email or credit card to access the application.</t>
+  </si>
+  <si>
+    <t>Factually correct information pertaining to physics fundementals displayed during runtime on the application.</t>
+  </si>
+  <si>
+    <t>Easy to understand UI interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A way to save specific results to come back to the same version of a problem at a later time without having to reset. Cookie based system stored locally. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Cookies to do anything malicious on end users computer. </t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1156,15 +1174,17 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="150" customHeight="1">
       <c r="A6" s="14" t="s">
@@ -1214,7 +1234,7 @@
     </row>
     <row r="9" spans="1:10" ht="150" customHeight="1">
       <c r="A9" s="14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>12</v>
@@ -1234,17 +1254,27 @@
       <c r="G9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="H9" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="128">
       <c r="A10" s="14"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="150" customHeight="1">
       <c r="A11" s="14" t="s">

</xml_diff>

<commit_message>
fixing formatting on spreadsheet
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCEB112-2123-C644-B42F-6330E81FFDDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46104038-1E3A-CD4F-A249-CAA9C7DAFDA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1093,7 +1093,7 @@
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1">
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="45" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
adding finished team txt file, adding team logo for project
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46104038-1E3A-CD4F-A249-CAA9C7DAFDA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B2DB23-671C-124D-AC1B-D98EE794F684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1062,7 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Attempt 1 at fix of corrupt file.
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -332,29 +332,30 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">A parking web application for students who have difficulty finding parking in and around campus. Prioritizing by time which lots will be open at any time to allow for efficient searching for parking in areas that may be less full at certain times in the day compared to others.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">A parking web application for students who have difficulty finding parking in and around campus. Prioritizing by time which lots will be open at any time to allow for efficient searching for parking in areas that may be less full at certain times in the day compared to others.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -514,9 +515,9 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -547,9 +548,9 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -580,9 +581,9 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -613,9 +614,9 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -811,9 +812,9 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
@@ -827,6 +828,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1156,7 +1158,7 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding updated spreadsheet with better formatting
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACD4CD0-87A1-EA48-819A-615A34ABD287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19360" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,26 +25,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
-  <si>
-    <t xml:space="preserve">&lt;CS3398 Kree Playing Poker Project Discussion&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project User Stories and Functional Requirements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planning Poker Ratings for Story</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional Components and Features of the Story</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+  <si>
+    <t>&lt;CS3398 Kree Playing Poker Project Discussion&gt;</t>
+  </si>
+  <si>
+    <t>Project User Stories and Functional Requirements</t>
+  </si>
+  <si>
+    <t>Author(s)</t>
+  </si>
+  <si>
+    <t>Planning Poker Ratings for Story</t>
+  </si>
+  <si>
+    <t>Functional Components and Features of the Story</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -56,11 +61,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Sam Pugh, David Kim, Shelby Jordan,</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t>Sam Pugh, David Kim, Shelby Jordan,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -77,11 +82,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ben Kownacki</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t>Ben Kownacki</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -94,7 +99,7 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -109,16 +114,15 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri (Body)"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Hi -&gt; More Interest)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(Hi -&gt; More Interest)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -133,56 +137,55 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri (Body)"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Hi -&gt; More Difficult)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Must Have</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Should Have</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Could Have</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Won't Have</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qualities you want your stories to have…..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I Sam, as a Mathematics , major have difficulties and struggle when first attempting to solve Calculus equations.This  Derivative/Integral Caluculator is meant to assist those who need to see step by step procedures in order to better understand the process which the</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sam Pugh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculation Engine that can evaulate derivatives and integrals depending on settings specified by the user.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Gui with buttons and ways for the end user to input the inforamtion.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error Checking on Input values to verify they are in correct format before starting processing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fairies living within the code.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(Hi -&gt; More Difficult)</t>
+    </r>
+  </si>
+  <si>
+    <t>Must Have</t>
+  </si>
+  <si>
+    <t>Should Have</t>
+  </si>
+  <si>
+    <t>Could Have</t>
+  </si>
+  <si>
+    <t>Won't Have</t>
+  </si>
+  <si>
+    <t>Qualities you want your stories to have…..</t>
+  </si>
+  <si>
+    <t>I Sam, as a Mathematics , major have difficulties and struggle when first attempting to solve Calculus equations.This  Derivative/Integral Caluculator is meant to assist those who need to see step by step procedures in order to better understand the process which the</t>
+  </si>
+  <si>
+    <t>Sam Pugh</t>
+  </si>
+  <si>
+    <t>Calculation Engine that can evaulate derivatives and integrals depending on settings specified by the user.</t>
+  </si>
+  <si>
+    <t>A Gui with buttons and ways for the end user to input the inforamtion.</t>
+  </si>
+  <si>
+    <t>Error Checking on Input values to verify they are in correct format before starting processing.</t>
+  </si>
+  <si>
+    <t>Fairies living within the code.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Independent:</t>
+      <t>Independent:</t>
     </r>
     <r>
       <rPr>
@@ -197,14 +200,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Negotiable:</t>
+      <t>Negotiable:</t>
     </r>
     <r>
       <rPr>
@@ -219,14 +222,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Valuable:</t>
+      <t>Valuable:</t>
     </r>
     <r>
       <rPr>
@@ -241,14 +244,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Estimable:</t>
+      <t>Estimable:</t>
     </r>
     <r>
       <rPr>
@@ -263,14 +266,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Small:</t>
+      <t>Small:</t>
     </r>
     <r>
       <rPr>
@@ -285,14 +288,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Testable:</t>
+      <t>Testable:</t>
     </r>
     <r>
       <rPr>
@@ -310,13 +313,13 @@
     <t xml:space="preserve">Must be integrated within a web application. </t>
   </si>
   <si>
-    <t xml:space="preserve">Methods showing the steps that are taking place throughout the calculations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional resource options if the student does not understand the steps.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Happy brithday playing whenever you git the calculate button.</t>
+    <t>Methods showing the steps that are taking place throughout the calculations.</t>
+  </si>
+  <si>
+    <t>Additional resource options if the student does not understand the steps.</t>
+  </si>
+  <si>
+    <t>Happy brithday playing whenever you git the calculate button.</t>
   </si>
   <si>
     <r>
@@ -347,7 +350,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">A parking web application for students who have difficulty finding parking in and around campus. Prioritizing by time which lots will be open at any time to allow for efficient searching for parking in areas that may be less full at certain times in the day compared to others.</t>
+      <t>A parking web application for students who have difficulty finding parking in and around campus. Prioritizing by time which lots will be open at any time to allow for efficient searching for parking in areas that may be less full at certain times in the day compared to others.</t>
     </r>
     <r>
       <rPr>
@@ -361,7 +364,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Shelby J</t>
+    <t>Shelby J</t>
   </si>
   <si>
     <r>
@@ -393,7 +396,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Will display best parking options based on estimated arrival time.</t>
+      <t>Will display best parking options based on estimated arrival time.</t>
     </r>
   </si>
   <si>
@@ -426,7 +429,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">Blacked out areas on the map to indicate no parking available.</t>
+      <t>Blacked out areas on the map to indicate no parking available.</t>
     </r>
   </si>
   <si>
@@ -459,11 +462,11 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">Interfaces with GPS application or Google Maps Web version.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Traffic indicators for road conditions i.e. display congested roads visually.
+      <t>Interfaces with GPS application or Google Maps Web version.</t>
+    </r>
+  </si>
+  <si>
+    <t>Traffic indicators for road conditions i.e. display congested roads visually.
 Include visitor parking spots at apartment complexes that are on the university bus route.
 Bus routes.</t>
   </si>
@@ -497,7 +500,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">A web application that displays the current total loans on your student account, how much interest is for each loan, the start date of the interest, and interest accrued to date.</t>
+      <t>A web application that displays the current total loans on your student account, how much interest is for each loan, the start date of the interest, and interest accrued to date.</t>
     </r>
   </si>
   <si>
@@ -530,7 +533,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">The ability to interact with multiple loaning companies to gather all the required information about the loans.</t>
+      <t>The ability to interact with multiple loaning companies to gather all the required information about the loans.</t>
     </r>
   </si>
   <si>
@@ -563,7 +566,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">An option to predict how much you will pay back to the loan depending on a variety of factors such as how much you want to pay monthly.</t>
+      <t>An option to predict how much you will pay back to the loan depending on a variety of factors such as how much you want to pay monthly.</t>
     </r>
   </si>
   <si>
@@ -596,7 +599,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">Integration with the TX State application.</t>
+      <t>Integration with the TX State application.</t>
     </r>
   </si>
   <si>
@@ -629,29 +632,29 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">The ability to change the loan amount; The ability to ask the provider of the loan for another loan.</t>
+      <t>The ability to change the loan amount; The ability to ask the provider of the loan for another loan.</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">I Sam, as a user who must take Physics to obtain my degree have trouble because the fundementals of Physics can be  frusterating for students who tend to be visual learners. This web application is meant to alleviate those troubles by adding graphics to the calculations to help students visualize the concepts by seeing graphics of how interactions of objects occur and the different forces/energies that they interact with as well as the objects themselves. </t>
   </si>
   <si>
-    <t xml:space="preserve">Beautiful UI Interface dependent on calculations from sliding bars indicating values.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efficient Methods to make calculations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ability to modify values on the fly to see the changes in real time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An email or credit card to access the application.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Factually correct information pertaining to physics fundementals displayed during runtime on the application.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easy to understand UI interface.</t>
+    <t>Beautiful UI Interface dependent on calculations from sliding bars indicating values.</t>
+  </si>
+  <si>
+    <t>Efficient Methods to make calculations.</t>
+  </si>
+  <si>
+    <t>Ability to modify values on the fly to see the changes in real time.</t>
+  </si>
+  <si>
+    <t>An email or credit card to access the application.</t>
+  </si>
+  <si>
+    <t>Factually correct information pertaining to physics fundementals displayed during runtime on the application.</t>
+  </si>
+  <si>
+    <t>Easy to understand UI interface.</t>
   </si>
   <si>
     <t xml:space="preserve">A way to save specific results to come back to the same version of a problem at a later time without having to reset. Cookie based system stored locally. </t>
@@ -663,46 +666,43 @@
     <t xml:space="preserve">I David, would like to prevent people's wifi getting hacked into and to be able to give them resources on how to have a seure network. The Wifi Password Cracker can be used to test wireless passwords and ensure they are secure enough to avoid others from connecting and stealing wireless internet. </t>
   </si>
   <si>
-    <t xml:space="preserve">David Kim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Successfully cracks into the wifi network and retrieve the password without causing any harm.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effective way to crack the network without being detected.</t>
+    <t>David Kim</t>
+  </si>
+  <si>
+    <t>Successfully cracks into the wifi network and retrieve the password without causing any harm.</t>
+  </si>
+  <si>
+    <t>Effective way to crack the network without being detected.</t>
   </si>
   <si>
     <t xml:space="preserve">Ability to get notified when password has been changed and retrieves the password immediatley </t>
   </si>
   <si>
-    <t xml:space="preserve">Crack wifi passwords with low signal or low user traffic.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I David, would like to help out people with disabilities. This  currency detector mobile app will allows the user to know how much money they're receiving and  have in their possession .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not Sumbitted For Rating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">App that can detect US currency and it's dollar amount.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Able to run the app purely on voice command.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automatically detect the currency and tell you the dollar amount when the user hovers their phone's camer over the money</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detailed UI.</t>
+    <t>Crack wifi passwords with low signal or low user traffic.</t>
+  </si>
+  <si>
+    <t>I David, would like to help out people with disabilities. This  currency detector mobile app will allows the user to know how much money they're receiving and  have in their possession .</t>
+  </si>
+  <si>
+    <t>Not Sumbitted For Rating</t>
+  </si>
+  <si>
+    <t>App that can detect US currency and it's dollar amount.</t>
+  </si>
+  <si>
+    <t>Able to run the app purely on voice command.</t>
+  </si>
+  <si>
+    <t>Automatically detect the currency and tell you the dollar amount when the user hovers their phone's camer over the money</t>
+  </si>
+  <si>
+    <t>Detailed UI.</t>
   </si>
   <si>
     <t xml:space="preserve">As an owner of one greedy and one dopey rat, I want to prevent the greedy rat from stealing food from the dopey one and hiding it on his level of the cage so I don't have to move around the food every couple of days.  </t>
   </si>
   <si>
-    <t xml:space="preserve">Ben Kownacki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Way to recognize when rat has food in its mouth, way to prevent that rat from moving up a level in the cage (arduino + servos).</t>
+    <t>Ben Kownacki</t>
   </si>
   <si>
     <t xml:space="preserve">Ability to determine food status based using AI. </t>
@@ -711,32 +711,47 @@
     <t xml:space="preserve">A way to tell each rat apart so we can allow the dopey rat up at all times, but prevent the greedy rat going up when he has food. </t>
   </si>
   <si>
-    <t xml:space="preserve">A GUI. Anything that could hurt or scare either rat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a construction documentation specialist who does a lot of picture manipulation, I want a tool that makes changing the order of JPG picture files and inserting pictures easier in the filesystem so that I don’t have to spend hours messing around with file names and non-specialized file renaming tools.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A great, easy to use, GUI. Ability to drag and drop pictures to change their order in the filesystem. An undo button.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ability to insert pictures or replace pictures with a marking placard with user-customizable text.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ability to reverse order of pictures, maniuplate order of a small subset of pictures, tool that automatically imports files from SD card, auto-rotates them, and inserts them into a new folder.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any type of AI or internet connectivity. A way to irreversibly mess up the order of photos in the filesystem. </t>
+    <t>As a construction documentation specialist who does a lot of picture manipulation, I want a tool that makes changing the order of JPG picture files and inserting pictures easier in the filesystem so that I don’t have to spend hours messing around with file names and non-specialized file renaming tools.</t>
+  </si>
+  <si>
+    <t>Ability to insert pictures or replace pictures with a marking placard with user-customizable text.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A great, easy to use, GUI. </t>
+  </si>
+  <si>
+    <t>Ability to drag and drop pictures to change their order in the filesystem. An undo button.</t>
+  </si>
+  <si>
+    <t>maniuplate order of a small subset of pictures, tool that automatically imports files from SD card, auto-rotates them, and inserts them into a new folder.</t>
+  </si>
+  <si>
+    <t>Ability to reverse order of pictures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any type of AI or internet connectivity. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A way to irreversibly mess up the order of photos in the filesystem. </t>
+  </si>
+  <si>
+    <t>Way to recognize when rat has food in its mouth.</t>
+  </si>
+  <si>
+    <t>way to prevent that rat from moving up a level in the cage (arduino + servos).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A GUI. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anything that could hurt or scare either rat.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="17">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -745,22 +760,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -768,7 +768,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -776,7 +776,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -794,7 +794,6 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -926,21 +925,29 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thick">
         <color rgb="FF1F4E79"/>
       </left>
@@ -955,7 +962,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thick">
         <color rgb="FF385724"/>
       </left>
@@ -969,125 +976,77 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1146,443 +1105,757 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F4E79"/>
       <rgbColor rgb="FF262626"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="49.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.83"/>
+    <col min="1" max="1" width="41.33203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+    <col min="10" max="10" width="49.33203125" customWidth="1"/>
+    <col min="11" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" s="8" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" s="12" customFormat="1" ht="45" customHeight="1">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="J2" s="9" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="J2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" s="8" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="10" t="s">
+    <row r="3" spans="1:10" s="12" customFormat="1" ht="43">
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="146" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:10" ht="146" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="14" t="n">
+      <c r="C4" s="18">
         <v>34</v>
       </c>
-      <c r="D4" s="14" t="n">
+      <c r="D4" s="18">
         <v>34</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15" t="s">
+    <row r="5" spans="1:10" ht="80">
+      <c r="A5" s="3"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
+    <row r="6" spans="1:10" ht="150" customHeight="1">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:10" ht="150" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="14" t="n">
+      <c r="C7" s="18">
         <v>55</v>
       </c>
-      <c r="D7" s="14" t="n">
+      <c r="D7" s="18">
         <v>55</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" customFormat="false" ht="166.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="s">
+    <row r="8" spans="1:10" ht="150" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:10" ht="167" customHeight="1">
+      <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="14" t="n">
+      <c r="C9" s="18">
         <v>21</v>
       </c>
-      <c r="D9" s="14" t="n">
+      <c r="D9" s="18">
         <v>13</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
+    <row r="10" spans="1:10" ht="150" customHeight="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="150" customHeight="1">
+      <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="14" t="n">
+      <c r="C11" s="18">
         <v>55</v>
       </c>
-      <c r="D11" s="14" t="n">
+      <c r="D11" s="18">
         <v>34</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="123.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15" t="s">
+    <row r="12" spans="1:10" ht="128">
+      <c r="A12" s="3"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
+    <row r="13" spans="1:10" ht="150" customHeight="1">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" ht="150" customHeight="1">
+      <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="14" t="n">
+      <c r="C14" s="18">
         <v>34</v>
       </c>
-      <c r="D14" s="14" t="n">
+      <c r="D14" s="18">
         <v>34</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" customFormat="false" ht="157" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+    <row r="15" spans="1:10" ht="150" customHeight="1">
+      <c r="A15" s="3"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" ht="157" customHeight="1">
+      <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
+    <row r="17" spans="1:8" ht="150" customHeight="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" ht="150" customHeight="1">
+      <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="G18" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="H18" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="150" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="150" customHeight="1">
+      <c r="A20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="B20" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="19" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15" t="s">
+      <c r="G20" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="150" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F21" s="19"/>
+      <c r="G21" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H21" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A15"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding updated spreadsheet with better formatting, split up single cell answers
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACD4CD0-87A1-EA48-819A-615A34ABD287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2AF594-954B-5749-93B0-B1CEBD392941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19360" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
   <si>
     <t>&lt;CS3398 Kree Playing Poker Project Discussion&gt;</t>
   </si>
@@ -367,275 +367,39 @@
     <t>Shelby J</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">As a Texas State University student, I want to be able to determine all the details about my education loans so that I can better plan my finances.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FF262626"/>
         <rFont val="Verdana"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Interactive UI that is up to date with current traffic and an interface for the user to specify estimated arrival times. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Will display best parking options based on estimated arrival time.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">Color coded map to indicate which parking lots are available based on type of parking pass.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>Blacked out areas on the map to indicate no parking available.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">Notification of any changes to estimated prediction. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>Interfaces with GPS application or Google Maps Web version.</t>
-    </r>
-  </si>
-  <si>
-    <t>Traffic indicators for road conditions i.e. display congested roads visually.
-Include visitor parking spots at apartment complexes that are on the university bus route.
-Bus routes.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">As a Texas State University student, I want to be able to determine all the details about my education loans so that I can better plan my finances.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
       <t>A web application that displays the current total loans on your student account, how much interest is for each loan, the start date of the interest, and interest accrued to date.</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">Easily navigable UI to identify each loan segment like the interest rate.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>The ability to interact with multiple loaning companies to gather all the required information about the loans.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">Breakdown of the loan, the amount due, and the due date.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>An option to predict how much you will pay back to the loan depending on a variety of factors such as how much you want to pay monthly.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">An option to predict how long it will take you to pay back the loan based on various inputs.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>Integration with the TX State application.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">The ability to make payments.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>The ability to change the loan amount; The ability to ask the provider of the loan for another loan.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">I Sam, as a user who must take Physics to obtain my degree have trouble because the fundementals of Physics can be  frusterating for students who tend to be visual learners. This web application is meant to alleviate those troubles by adding graphics to the calculations to help students visualize the concepts by seeing graphics of how interactions of objects occur and the different forces/energies that they interact with as well as the objects themselves. </t>
   </si>
   <si>
@@ -745,13 +509,61 @@
   </si>
   <si>
     <t xml:space="preserve"> Anything that could hurt or scare either rat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactive UI that is up to date with current traffic and an interface for the user to specify estimated arrival times. </t>
+  </si>
+  <si>
+    <t>Will display best parking options based on estimated arrival time.</t>
+  </si>
+  <si>
+    <t>Color coded map to indicate which parking lots are available based on type of parking pass.</t>
+  </si>
+  <si>
+    <t>Blacked out areas on the map to indicate no parking available</t>
+  </si>
+  <si>
+    <t>Interfaces with GPS application or Google Maps Web version.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notification of any changes to estimated prediction. </t>
+  </si>
+  <si>
+    <t>Include visitor parking spots at apartment complexes that are on the university bus route.</t>
+  </si>
+  <si>
+    <t>Traffic indicators for road conditions i.e. display congested roads visually.</t>
+  </si>
+  <si>
+    <t>Easily navigable UI to identify each loan segment like the interest rate.</t>
+  </si>
+  <si>
+    <t>The ability to interact with multiple loaning companies to gather all the required information about the loans.</t>
+  </si>
+  <si>
+    <t>Breakdown of the loan, the amount due, and the due date.</t>
+  </si>
+  <si>
+    <t>An option to predict how much you will pay back to the loan depending on a variety of factors such as how much you want to pay monthly.</t>
+  </si>
+  <si>
+    <t>Integration with the TX State application.</t>
+  </si>
+  <si>
+    <t>An option to predict how long it will take you to pay back the loan based on various inputs.</t>
+  </si>
+  <si>
+    <t>The ability to change the loan amount; The ability to ask the provider of the loan for another loan.</t>
+  </si>
+  <si>
+    <t>The ability to make payments.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -832,12 +644,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF262626"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1038,7 +844,7 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1425,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1550,305 +1356,312 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="150" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="18">
+        <v>55</v>
+      </c>
+      <c r="D6" s="18">
+        <v>55</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="150" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="150" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C8" s="18">
+        <v>21</v>
+      </c>
+      <c r="D8" s="18">
+        <v>13</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="167" customHeight="1">
+      <c r="A9" s="1"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="150" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="18">
         <v>55</v>
       </c>
-      <c r="D7" s="18">
-        <v>55</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="22" t="s">
+      <c r="D10" s="18">
+        <v>34</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="F10" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="150" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-    </row>
-    <row r="9" spans="1:10" ht="167" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="G10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="18">
-        <v>21</v>
-      </c>
-      <c r="D9" s="18">
-        <v>13</v>
-      </c>
-      <c r="E9" s="22" t="s">
+      <c r="H10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="22" t="s">
+    </row>
+    <row r="11" spans="1:10" ht="150" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="F11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="G11" s="19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="150" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-    </row>
-    <row r="11" spans="1:10" ht="150" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="H11" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="18">
-        <v>55</v>
-      </c>
-      <c r="D11" s="18">
-        <v>34</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="128">
-      <c r="A12" s="3"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="16"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" ht="150" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="18">
+        <v>34</v>
+      </c>
+      <c r="D13" s="18">
+        <v>34</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="H13" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="19" t="s">
+    </row>
+    <row r="14" spans="1:10" ht="150" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" ht="150" customHeight="1">
+      <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="B15" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="150" customHeight="1">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:10" ht="150" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="D15" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="F15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="18">
-        <v>34</v>
-      </c>
-      <c r="D14" s="18">
-        <v>34</v>
-      </c>
-      <c r="E14" s="19" t="s">
+      <c r="G15" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="H15" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="19" t="s">
+    </row>
+    <row r="16" spans="1:10" ht="157" customHeight="1">
+      <c r="A16" s="3"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:8" ht="150" customHeight="1">
+      <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="B17" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="150" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:10" ht="157" customHeight="1">
-      <c r="A16" s="3" t="s">
+      <c r="C17" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="18" t="s">
+      <c r="G17" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="H17" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="150" customHeight="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="150" customHeight="1">
+      <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="B19" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="19" t="s">
+      <c r="G19" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="150" customHeight="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="150" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="1:8" ht="150" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="19" t="s">
+      <c r="H20" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="H18" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="150" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="150" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="150" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
+    </row>
+    <row r="21" spans="1:8" ht="150" customHeight="1"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>

</xml_diff>

<commit_message>
adding updated spreadsheet with Jessee Ideas
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2AF594-954B-5749-93B0-B1CEBD392941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FA32B8-EDB7-4C43-8B72-77B01829F184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19360" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11900" yWindow="460" windowWidth="19360" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="99">
   <si>
     <t>&lt;CS3398 Kree Playing Poker Project Discussion&gt;</t>
   </si>
@@ -40,61 +40,6 @@
   </si>
   <si>
     <t>Functional Components and Features of the Story</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">List Team Members Here: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Sam Pugh, David Kim, Shelby Jordan,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Ben Kownacki</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
   </si>
   <si>
     <r>
@@ -557,6 +502,110 @@
   </si>
   <si>
     <t>The ability to make payments.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">List Team Members Here: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Sam Pugh, David Kim, Shelby Jordan,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Ben Kownacki</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+  </si>
+  <si>
+    <t>As a computer scientist i believe we should be constantly looking for ways that can benefit others especially when it comes to those that have disabilities and this project would help people with different dissablities. An application that follows eye movement to operate the computer like the mouse does.</t>
+  </si>
+  <si>
+    <t>Jesse Munoz</t>
+  </si>
+  <si>
+    <t>A way to track eyes.</t>
+  </si>
+  <si>
+    <t>A menu to do things easier such as esc, enter, etc.</t>
+  </si>
+  <si>
+    <t>options to learn and adapt from the way the user specifically does things.</t>
+  </si>
+  <si>
+    <t>A way to click in a fast manner</t>
+  </si>
+  <si>
+    <t>A way to click things by either blinking or staring at option for a given time.</t>
+  </si>
+  <si>
+    <t>Not able to track other peoples eyes.</t>
+  </si>
+  <si>
+    <t>A separate piece of equipment that could be used to help track eye movement</t>
+  </si>
+  <si>
+    <t>A way to type fast</t>
+  </si>
+  <si>
+    <t>As a student who doesnt take well notes this application would benefit me but also from seeing other college students i could see this program benefit others as well. Students miss class or just dont do well at taking notes and this program could help a lot of students. An application just for Texas state students to put up old notes to use for other texas state students to benefit from</t>
+  </si>
+  <si>
+    <t>A way to upload notes online and sort through what is trash and what is actual notes</t>
+  </si>
+  <si>
+    <t>A way to sort the notes for which classes and sort them based off best relevance for what the user looks up</t>
+  </si>
+  <si>
+    <t>A way to subscirbe to note takers that the user believes takes really good notes.</t>
+  </si>
+  <si>
+    <t>A way to edit the notes.</t>
+  </si>
+  <si>
+    <t>A way to download the notes.</t>
+  </si>
+  <si>
+    <t>A way to vote up or down on notes to determine if the notes are good for others to see.</t>
+  </si>
+  <si>
+    <t>A way to determine that none of the notes contain just answers to questions that would be assoicated with cheating</t>
+  </si>
+  <si>
+    <t>A way to cheat.</t>
   </si>
 </sst>
 </file>
@@ -730,7 +779,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -781,11 +830,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -826,9 +901,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -845,6 +917,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1229,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1280,388 +1364,463 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="J2" s="13" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" ht="43">
       <c r="A3" s="7"/>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="J3" s="15" t="s">
         <v>11</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="146" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="17">
+        <v>34</v>
+      </c>
+      <c r="D4" s="17">
+        <v>34</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="18">
-        <v>34</v>
-      </c>
-      <c r="D4" s="18">
-        <v>34</v>
-      </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="J4" s="19" t="s">
         <v>18</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="80">
       <c r="A5" s="3"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="150" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>55</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>55</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>71</v>
+      <c r="E6" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="150" customHeight="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="19" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>70</v>
+      <c r="H7" s="18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="18">
+      <c r="B8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="17">
         <v>21</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>13</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>79</v>
+      <c r="E8" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="167" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="19" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>78</v>
+      <c r="H9" s="18" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="150" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="17">
+        <v>55</v>
+      </c>
+      <c r="D10" s="17">
+        <v>34</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="18">
-        <v>55</v>
-      </c>
-      <c r="D10" s="18">
-        <v>34</v>
-      </c>
-      <c r="E10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="G10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="H10" s="18" t="s">
         <v>30</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="150" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="19" t="s">
+    </row>
+    <row r="12" spans="1:10" ht="96">
+      <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="B12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="17">
+        <v>34</v>
+      </c>
+      <c r="D12" s="17">
+        <v>34</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="150" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" ht="150" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="18">
-        <v>34</v>
-      </c>
-      <c r="D13" s="18">
-        <v>34</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="150" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="C14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="150" customHeight="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" ht="157" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="157" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="D16" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="150" customHeight="1">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="150" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="150" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19" t="s">
-        <v>63</v>
+      <c r="C18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="150" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="19" t="s">
+      <c r="A19" s="3"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="H19" s="19" t="s">
+      <c r="F19" s="18"/>
+      <c r="G19" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="18" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="150" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="150" customHeight="1"/>
+      <c r="A20" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="150" customHeight="1">
+      <c r="A21" s="24"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="150" customHeight="1">
+      <c r="A22" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="150" customHeight="1">
+      <c r="A23" s="25"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
+  <mergeCells count="15">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>

</xml_diff>

<commit_message>
adding david's additions to spreadsheet
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FA32B8-EDB7-4C43-8B72-77B01829F184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F311BF7E-10E1-884B-A519-F5002451D162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11900" yWindow="460" windowWidth="19360" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19360" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
   <si>
     <t>&lt;CS3398 Kree Playing Poker Project Discussion&gt;</t>
   </si>
@@ -606,6 +606,27 @@
   </si>
   <si>
     <t>A way to cheat.</t>
+  </si>
+  <si>
+    <t>Be able to send password change request or alerts about the network.</t>
+  </si>
+  <si>
+    <t>A GUI to show how strong the wifi connection is.</t>
+  </si>
+  <si>
+    <t>Able to block user from changing password.</t>
+  </si>
+  <si>
+    <t>Mobile phone access</t>
+  </si>
+  <si>
+    <t>Easy to use format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Able to differentiate US currency and other countries currency. </t>
+  </si>
+  <si>
+    <t>Any functions or features that require payments.</t>
   </si>
 </sst>
 </file>
@@ -862,30 +883,6 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -919,17 +916,41 @@
     <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1315,13 +1336,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
@@ -1334,498 +1355,514 @@
     <col min="11" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="42" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="42" customHeight="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" s="12" customFormat="1" ht="45" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="J2" s="13" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="J2" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="12" customFormat="1" ht="43">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="14" t="s">
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="43">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="146" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="9">
         <v>34</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="9">
         <v>34</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="80">
-      <c r="A5" s="3"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="150" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="9">
         <v>55</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="9">
         <v>55</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="150" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="9">
         <v>21</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="9">
         <v>13</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="167" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="150" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="9">
         <v>55</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="9">
         <v>34</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="150" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="96">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="9">
         <v>34</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="9">
         <v>34</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="150" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="150" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="150" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="157" customHeight="1">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="150" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18" t="s">
+      <c r="A17" s="15"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="150" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="150" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="150" customHeight="1">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="150" customHeight="1">
-      <c r="A21" s="24"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="10" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="150" customHeight="1">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="150" customHeight="1">
-      <c r="A23" s="25"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="10" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
packaging for final submission
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
+++ b/Assignments/Assignment_4/Kree_User_Story_Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F311BF7E-10E1-884B-A519-F5002451D162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D51799-5F04-3E42-837F-AD980113B537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19360" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6240" yWindow="460" windowWidth="19360" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="108">
   <si>
     <t>&lt;CS3398 Kree Playing Poker Project Discussion&gt;</t>
   </si>
@@ -265,48 +265,6 @@
   </si>
   <si>
     <t>Happy brithday playing whenever you git the calculate button.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">As a Texas State student, I want to be able to find out where I can park on the University so that I don’t spend unnecessary time searching for parking. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>A parking web application for students who have difficulty finding parking in and around campus. Prioritizing by time which lots will be open at any time to allow for efficient searching for parking in areas that may be less full at certain times in the day compared to others.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
   </si>
   <si>
     <t>Shelby J</t>
@@ -504,6 +462,126 @@
     <t>The ability to make payments.</t>
   </si>
   <si>
+    <t>As a computer scientist i believe we should be constantly looking for ways that can benefit others especially when it comes to those that have disabilities and this project would help people with different dissablities. An application that follows eye movement to operate the computer like the mouse does.</t>
+  </si>
+  <si>
+    <t>Jesse Munoz</t>
+  </si>
+  <si>
+    <t>A way to track eyes.</t>
+  </si>
+  <si>
+    <t>A menu to do things easier such as esc, enter, etc.</t>
+  </si>
+  <si>
+    <t>options to learn and adapt from the way the user specifically does things.</t>
+  </si>
+  <si>
+    <t>A way to click in a fast manner</t>
+  </si>
+  <si>
+    <t>A way to click things by either blinking or staring at option for a given time.</t>
+  </si>
+  <si>
+    <t>Not able to track other peoples eyes.</t>
+  </si>
+  <si>
+    <t>A separate piece of equipment that could be used to help track eye movement</t>
+  </si>
+  <si>
+    <t>A way to type fast</t>
+  </si>
+  <si>
+    <t>As a student who doesnt take well notes this application would benefit me but also from seeing other college students i could see this program benefit others as well. Students miss class or just dont do well at taking notes and this program could help a lot of students. An application just for Texas state students to put up old notes to use for other texas state students to benefit from</t>
+  </si>
+  <si>
+    <t>A way to upload notes online and sort through what is trash and what is actual notes</t>
+  </si>
+  <si>
+    <t>A way to sort the notes for which classes and sort them based off best relevance for what the user looks up</t>
+  </si>
+  <si>
+    <t>A way to subscirbe to note takers that the user believes takes really good notes.</t>
+  </si>
+  <si>
+    <t>A way to edit the notes.</t>
+  </si>
+  <si>
+    <t>A way to download the notes.</t>
+  </si>
+  <si>
+    <t>A way to vote up or down on notes to determine if the notes are good for others to see.</t>
+  </si>
+  <si>
+    <t>A way to determine that none of the notes contain just answers to questions that would be assoicated with cheating</t>
+  </si>
+  <si>
+    <t>A way to cheat.</t>
+  </si>
+  <si>
+    <t>Be able to send password change request or alerts about the network.</t>
+  </si>
+  <si>
+    <t>A GUI to show how strong the wifi connection is.</t>
+  </si>
+  <si>
+    <t>Able to block user from changing password.</t>
+  </si>
+  <si>
+    <t>Mobile phone access</t>
+  </si>
+  <si>
+    <t>Easy to use format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Able to differentiate US currency and other countries currency. </t>
+  </si>
+  <si>
+    <t>Any functions or features that require payments.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a Texas State student, I want to be able to find out where I can park on the University so that I don’t spend unnecessary time searching for parking. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>A parking web application for students who have difficulty finding parking in and around campus. Prioritizing by time which lots will be open at any time to allow for efficient searching for parking in areas that may be less full at certain times in the day compared to others.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Ability to manipulate order of a small subset of pictures, tool that automatically imports files from SD card.</t>
+  </si>
+  <si>
+    <t>Minimal error rate so greedy rat can always access his food when he needs to.</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">List Team Members Here: </t>
     </r>
@@ -540,100 +618,20 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-  </si>
-  <si>
-    <t>As a computer scientist i believe we should be constantly looking for ways that can benefit others especially when it comes to those that have disabilities and this project would help people with different dissablities. An application that follows eye movement to operate the computer like the mouse does.</t>
-  </si>
-  <si>
-    <t>Jesse Munoz</t>
-  </si>
-  <si>
-    <t>A way to track eyes.</t>
-  </si>
-  <si>
-    <t>A menu to do things easier such as esc, enter, etc.</t>
-  </si>
-  <si>
-    <t>options to learn and adapt from the way the user specifically does things.</t>
-  </si>
-  <si>
-    <t>A way to click in a fast manner</t>
-  </si>
-  <si>
-    <t>A way to click things by either blinking or staring at option for a given time.</t>
-  </si>
-  <si>
-    <t>Not able to track other peoples eyes.</t>
-  </si>
-  <si>
-    <t>A separate piece of equipment that could be used to help track eye movement</t>
-  </si>
-  <si>
-    <t>A way to type fast</t>
-  </si>
-  <si>
-    <t>As a student who doesnt take well notes this application would benefit me but also from seeing other college students i could see this program benefit others as well. Students miss class or just dont do well at taking notes and this program could help a lot of students. An application just for Texas state students to put up old notes to use for other texas state students to benefit from</t>
-  </si>
-  <si>
-    <t>A way to upload notes online and sort through what is trash and what is actual notes</t>
-  </si>
-  <si>
-    <t>A way to sort the notes for which classes and sort them based off best relevance for what the user looks up</t>
-  </si>
-  <si>
-    <t>A way to subscirbe to note takers that the user believes takes really good notes.</t>
-  </si>
-  <si>
-    <t>A way to edit the notes.</t>
-  </si>
-  <si>
-    <t>A way to download the notes.</t>
-  </si>
-  <si>
-    <t>A way to vote up or down on notes to determine if the notes are good for others to see.</t>
-  </si>
-  <si>
-    <t>A way to determine that none of the notes contain just answers to questions that would be assoicated with cheating</t>
-  </si>
-  <si>
-    <t>A way to cheat.</t>
-  </si>
-  <si>
-    <t>Be able to send password change request or alerts about the network.</t>
-  </si>
-  <si>
-    <t>A GUI to show how strong the wifi connection is.</t>
-  </si>
-  <si>
-    <t>Able to block user from changing password.</t>
-  </si>
-  <si>
-    <t>Mobile phone access</t>
-  </si>
-  <si>
-    <t>Easy to use format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Able to differentiate US currency and other countries currency. </t>
-  </si>
-  <si>
-    <t>Any functions or features that require payments.</t>
+      </rPr>
+      <t>, Jesse Munoz</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -724,6 +722,19 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -878,8 +889,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -953,7 +965,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{F0197539-1C0F-354F-8C41-E1FBDE38D8FD}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1337,7 +1350,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1385,7 +1398,7 @@
       <c r="G2" s="25"/>
       <c r="H2" s="25"/>
       <c r="J2" s="5" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" ht="43">
@@ -1462,10 +1475,10 @@
     </row>
     <row r="6" spans="1:10" ht="150" customHeight="1">
       <c r="A6" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="C6" s="9">
         <v>55</v>
@@ -1474,16 +1487,16 @@
         <v>55</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="150" customHeight="1">
@@ -1492,24 +1505,24 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="H7" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="9">
         <v>21</v>
@@ -1518,16 +1531,16 @@
         <v>13</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="167" customHeight="1">
@@ -1536,21 +1549,21 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="H9" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="150" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>13</v>
@@ -1562,16 +1575,16 @@
         <v>34</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="150" customHeight="1">
@@ -1580,24 +1593,24 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="96">
       <c r="A12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="C12" s="9">
         <v>34</v>
@@ -1606,16 +1619,16 @@
         <v>34</v>
       </c>
       <c r="E12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="150" customHeight="1">
@@ -1624,42 +1637,42 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="150" customHeight="1">
       <c r="A14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="150" customHeight="1">
@@ -1668,42 +1681,42 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>103</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="157" customHeight="1">
       <c r="A16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="H16" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="150" customHeight="1">
@@ -1712,38 +1725,42 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="H17" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="150" customHeight="1">
       <c r="A18" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="G18" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="150" customHeight="1">
@@ -1752,38 +1769,42 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="H19" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="150" customHeight="1">
       <c r="A20" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="F20" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="H20" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="150" customHeight="1">
@@ -1792,40 +1813,42 @@
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="H21" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="150" customHeight="1">
       <c r="A22" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10" t="s">
+      <c r="G22" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="H22" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="150" customHeight="1">
@@ -1834,16 +1857,16 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="H23" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>